<commit_message>
neue files mit den tablen für alle Einkommen, nicht nur die positiven
</commit_message>
<xml_diff>
--- a/reports/GBR/voting_detail.xlsx
+++ b/reports/GBR/voting_detail.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linokungl/Desktop/EconIneq/Ineq_project/reports/GBR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43483DF5-223E-F642-ABA4-316701CE8C25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BCF45-5CAE-CA47-880B-70FD629F2ADF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="14540" xr2:uid="{D600F15A-1C03-4142-8159-B74CC6D4513A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Region</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>North Eastern Scotland</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>UKE2</t>
@@ -273,7 +270,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,9 +308,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,21 +628,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94B2B63-3AE1-B144-9949-44E2A4E78E03}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -650,7 +651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -665,7 +666,7 @@
         <v>0.48070000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -680,7 +681,7 @@
         <v>0.53160000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -695,7 +696,7 @@
         <v>0.48329999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -710,7 +711,7 @@
         <v>0.43540000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -725,7 +726,7 @@
         <v>0.43569999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -740,7 +741,7 @@
         <v>0.41469999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -755,7 +756,7 @@
         <v>0.4466</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -770,7 +771,7 @@
         <v>0.43799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -785,7 +786,7 @@
         <v>0.44550000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -800,7 +801,7 @@
         <v>0.49750000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -815,7 +816,7 @@
         <v>0.35250000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -830,7 +831,7 @@
         <v>0.63179999999999992</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -845,7 +846,7 @@
         <v>0.37660000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -860,7 +861,7 @@
         <v>0.50879999999999992</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -875,7 +876,7 @@
         <v>0.46540000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -890,7 +891,7 @@
         <v>0.45420000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -905,7 +906,7 @@
         <v>0.43440000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -920,7 +921,7 @@
         <v>0.56040000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -935,7 +936,7 @@
         <v>0.71910000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -950,7 +951,7 @@
         <v>0.40749999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -965,7 +966,7 @@
         <v>0.40969999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -980,7 +981,7 @@
         <v>0.40969999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -995,7 +996,7 @@
         <v>0.34840000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1010,26 +1011,26 @@
         <v>0.51180000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2">
+        <v>0.42369959987688521</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.57630040012311479</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17">
+      <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C27">
         <v>0.51890000000000003</v>
@@ -1039,12 +1040,12 @@
         <v>0.48109999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17">
       <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C28">
         <v>0.44240000000000002</v>
@@ -1054,12 +1055,12 @@
         <v>0.55759999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17">
       <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C29">
         <v>0.55710000000000004</v>
@@ -1069,12 +1070,12 @@
         <v>0.44289999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17">
       <c r="A30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C30">
         <v>0.43969999999999998</v>
@@ -1084,12 +1085,12 @@
         <v>0.56030000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17">
       <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C31">
         <v>0.62529999999999997</v>
@@ -1099,12 +1100,12 @@
         <v>0.37470000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17">
       <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C32">
         <v>0.36780000000000002</v>
@@ -1114,12 +1115,12 @@
         <v>0.63219999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17">
       <c r="A33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C33">
         <v>0.61560000000000004</v>
@@ -1129,12 +1130,12 @@
         <v>0.38439999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17">
       <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C34">
         <v>0.4929</v>
@@ -1144,12 +1145,12 @@
         <v>0.5071</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17">
       <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C35">
         <v>0.6089</v>
@@ -1159,12 +1160,12 @@
         <v>0.3911</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17">
       <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C36">
         <v>0.58640000000000003</v>
@@ -1174,12 +1175,12 @@
         <v>0.41359999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17">
       <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C37">
         <v>0.53890000000000005</v>
@@ -1189,12 +1190,12 @@
         <v>0.46109999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17">
       <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C38">
         <v>0.54779999999999995</v>

</xml_diff>

<commit_message>
dummies für regionen eingefügt
</commit_message>
<xml_diff>
--- a/reports/GBR/voting_detail.xlsx
+++ b/reports/GBR/voting_detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linokungl/Desktop/EconIneq/Ineq_project/reports/GBR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BCF45-5CAE-CA47-880B-70FD629F2ADF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2538BA3-9CA0-F645-A718-59029FB6C464}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="14540" xr2:uid="{D600F15A-1C03-4142-8159-B74CC6D4513A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Region</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>Region Name</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Northern.Ireland</t>
+  </si>
+  <si>
+    <t>London</t>
   </si>
 </sst>
 </file>
@@ -271,7 +280,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -311,7 +320,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94B2B63-3AE1-B144-9949-44E2A4E78E03}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -637,7 +646,7 @@
     <col min="2" max="2" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -650,8 +659,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17">
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -665,8 +683,17 @@
         <f>1-C2</f>
         <v>0.48070000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -680,8 +707,17 @@
         <f t="shared" ref="D3:D38" si="0">1-C3</f>
         <v>0.53160000000000007</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -695,8 +731,17 @@
         <f t="shared" si="0"/>
         <v>0.48329999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -710,8 +755,17 @@
         <f t="shared" si="0"/>
         <v>0.43540000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -725,8 +779,17 @@
         <f t="shared" si="0"/>
         <v>0.43569999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -740,8 +803,17 @@
         <f t="shared" si="0"/>
         <v>0.41469999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -755,8 +827,17 @@
         <f t="shared" si="0"/>
         <v>0.4466</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -770,8 +851,17 @@
         <f t="shared" si="0"/>
         <v>0.43799999999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -785,8 +875,17 @@
         <f t="shared" si="0"/>
         <v>0.44550000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="17">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -800,8 +899,17 @@
         <f t="shared" si="0"/>
         <v>0.49750000000000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -815,8 +923,17 @@
         <f t="shared" si="0"/>
         <v>0.35250000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -830,8 +947,17 @@
         <f t="shared" si="0"/>
         <v>0.63179999999999992</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -845,8 +971,17 @@
         <f t="shared" si="0"/>
         <v>0.37660000000000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -860,8 +995,17 @@
         <f t="shared" si="0"/>
         <v>0.50879999999999992</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -875,8 +1019,17 @@
         <f t="shared" si="0"/>
         <v>0.46540000000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -890,8 +1043,17 @@
         <f t="shared" si="0"/>
         <v>0.45420000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -905,8 +1067,17 @@
         <f t="shared" si="0"/>
         <v>0.43440000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -920,8 +1091,17 @@
         <f t="shared" si="0"/>
         <v>0.56040000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -935,8 +1115,17 @@
         <f t="shared" si="0"/>
         <v>0.71910000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="17">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -950,8 +1139,17 @@
         <f t="shared" si="0"/>
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -965,8 +1163,17 @@
         <f t="shared" si="0"/>
         <v>0.40969999999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="17">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -980,8 +1187,17 @@
         <f t="shared" si="0"/>
         <v>0.40969999999999995</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="17">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -995,8 +1211,17 @@
         <f t="shared" si="0"/>
         <v>0.34840000000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="17">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1010,8 +1235,17 @@
         <f t="shared" si="0"/>
         <v>0.51180000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="17">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1024,8 +1258,17 @@
       <c r="D26" s="2">
         <v>0.57630040012311479</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="17">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1039,8 +1282,17 @@
         <f t="shared" si="0"/>
         <v>0.48109999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1054,8 +1306,17 @@
         <f t="shared" si="0"/>
         <v>0.55759999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1069,8 +1330,17 @@
         <f t="shared" si="0"/>
         <v>0.44289999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -1084,8 +1354,17 @@
         <f t="shared" si="0"/>
         <v>0.56030000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="17">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1099,8 +1378,17 @@
         <f t="shared" si="0"/>
         <v>0.37470000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1114,8 +1402,17 @@
         <f t="shared" si="0"/>
         <v>0.63219999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1129,8 +1426,17 @@
         <f t="shared" si="0"/>
         <v>0.38439999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1144,8 +1450,17 @@
         <f t="shared" si="0"/>
         <v>0.5071</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1159,8 +1474,17 @@
         <f t="shared" si="0"/>
         <v>0.3911</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="17">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1174,8 +1498,17 @@
         <f t="shared" si="0"/>
         <v>0.41359999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="17">
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17">
       <c r="A37" s="1" t="s">
         <v>73</v>
       </c>
@@ -1189,8 +1522,17 @@
         <f t="shared" si="0"/>
         <v>0.46109999999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17">
       <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
@@ -1203,6 +1545,15 @@
       <c r="D38">
         <f t="shared" si="0"/>
         <v>0.45220000000000005</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>